<commit_message>
modified:   Projet-Site Web-Grille de planification.xlsx 	modified:   README.md 	new file:   html/clothing.html 	new file:   html/contact.html 	new file:   html/gloves.html 	modified:   html/index.html 	new file:   html/mattress-organic.html 	new file:   html/mattress-pillows.html 	new file:   html/medical.html
</commit_message>
<xml_diff>
--- a/Projet-Site Web-Grille de planification.xlsx
+++ b/Projet-Site Web-Grille de planification.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ccnbca-my.sharepoint.com/personal/dimitri_viel_ccnb_ca/Documents/Prog1343/Lab4 - Vanderlay Industries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kamal\Documents\CCNB\HTML_PROG1343\LABs\LAB4\Lab4-VanderlayIndustries-G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{70D9F1CF-C19D-495D-9CA6-F522F37EBA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E3551A3-0986-4D72-93FD-E4C19105CB9D}"/>
   <bookViews>
-    <workbookView xWindow="4212" yWindow="3060" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="3060" windowWidth="17280" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
   <si>
     <t>Grille d'analyse pour le développement d'un site web</t>
   </si>
@@ -287,14 +286,56 @@
       <t xml:space="preserve">      Offrir des services (  )           Faire des ventes ( X )</t>
     </r>
   </si>
+  <si>
+    <t>ACCUEIL</t>
+  </si>
+  <si>
+    <t>GANTS EN LATEX</t>
+  </si>
+  <si>
+    <t>../html/gloves.html</t>
+  </si>
+  <si>
+    <t>../html/index.html</t>
+  </si>
+  <si>
+    <t>VÊTEMENTS LATEX</t>
+  </si>
+  <si>
+    <t>../html/clothing.html</t>
+  </si>
+  <si>
+    <t>MATELAS EN LATEX -&gt; Oreillers biologiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATELAS EN LATEX -&gt; Matelas biologique  </t>
+  </si>
+  <si>
+    <t>../html/mattress-organic.html</t>
+  </si>
+  <si>
+    <t>../html/mattress-pillows.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUITS MÉDICAUX LATEX </t>
+  </si>
+  <si>
+    <t>../html/medical.html</t>
+  </si>
+  <si>
+    <t>NOUS CONTACTER</t>
+  </si>
+  <si>
+    <t>../html/contact.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-1009]d/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-1009]d/mmm/yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -501,7 +542,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
@@ -545,13 +586,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -590,7 +631,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -605,12 +646,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -629,22 +679,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
+    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -917,42 +958,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="72.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>2</v>
       </c>
@@ -962,7 +1003,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>3</v>
       </c>
@@ -970,7 +1011,7 @@
       <c r="C6" s="33"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
@@ -980,7 +1021,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>5</v>
       </c>
@@ -988,7 +1029,7 @@
       <c r="C8" s="33"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>6</v>
       </c>
@@ -998,7 +1039,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>7</v>
       </c>
@@ -1008,53 +1049,53 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="38"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="14"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>15</v>
       </c>
@@ -1062,31 +1103,31 @@
       <c r="C16" s="33"/>
       <c r="D16" s="16"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="D20" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
+    <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>18</v>
       </c>
@@ -1096,27 +1137,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-    </row>
-    <row r="26" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+    </row>
+    <row r="26" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>21</v>
       </c>
@@ -1124,7 +1165,7 @@
       <c r="C26" s="33"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>22</v>
       </c>
@@ -1132,7 +1173,7 @@
       <c r="C27" s="33"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1181,7 @@
       <c r="C28" s="33"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>24</v>
       </c>
@@ -1150,37 +1191,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="42" t="s">
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="43"/>
-      <c r="C33" s="44"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="24" t="s">
         <v>28</v>
@@ -1188,7 +1229,7 @@
       <c r="C34" s="25"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="24" t="s">
         <v>29</v>
@@ -1198,7 +1239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="24" t="s">
         <v>31</v>
@@ -1206,7 +1247,7 @@
       <c r="C36" s="25"/>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="24" t="s">
         <v>32</v>
@@ -1214,7 +1255,7 @@
       <c r="C37" s="25"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>33</v>
       </c>
@@ -1224,7 +1265,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
         <v>35</v>
       </c>
@@ -1232,50 +1273,50 @@
       <c r="C39" s="33"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="40"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="35" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="45" t="s">
+    <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="45" t="s">
+    <row r="45" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1324,7 @@
       <c r="C46" s="33"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>41</v>
       </c>
@@ -1291,25 +1332,25 @@
       <c r="C47" s="33"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35" t="s">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-    </row>
-    <row r="51" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+    </row>
+    <row r="51" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>43</v>
       </c>
@@ -1319,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
         <v>44</v>
       </c>
@@ -1329,74 +1370,105 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="26">
         <v>2</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="26">
         <v>3</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="26">
         <v>4</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="26">
         <v>5</v>
       </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="26">
         <v>6</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="26">
         <v>7</v>
       </c>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="26">
         <v>8</v>
       </c>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="26">
         <v>9</v>
       </c>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="26">
         <v>10</v>
@@ -1404,7 +1476,7 @@
       <c r="C62" s="20"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="26">
         <v>11</v>
@@ -1412,7 +1484,7 @@
       <c r="C63" s="20"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="26">
         <v>12</v>
@@ -1420,7 +1492,7 @@
       <c r="C64" s="20"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
         <v>46</v>
       </c>
@@ -1428,7 +1500,7 @@
       <c r="C65" s="33"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
         <v>47</v>
       </c>
@@ -1438,7 +1510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
         <v>49</v>
       </c>
@@ -1446,55 +1518,55 @@
       <c r="C67" s="33"/>
       <c r="D67" s="31"/>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="35" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-    </row>
-    <row r="71" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="36" t="s">
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+    </row>
+    <row r="71" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B71" s="37"/>
-      <c r="C71" s="38"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="41"/>
       <c r="D71" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="36" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B72" s="37"/>
-      <c r="C72" s="38"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="41"/>
       <c r="D72" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="36" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B73" s="37"/>
-      <c r="C73" s="38"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="41"/>
       <c r="D73" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
         <v>54</v>
       </c>
@@ -1504,7 +1576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
         <v>55</v>
       </c>
@@ -1514,7 +1586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
         <v>56</v>
       </c>
@@ -1524,20 +1596,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="19"/>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="35" t="s">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-    </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+    </row>
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
         <v>58</v>
       </c>
@@ -1545,7 +1617,7 @@
       <c r="C79" s="33"/>
       <c r="D79" s="29"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
         <v>59</v>
       </c>
@@ -1555,7 +1627,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
       <c r="B81" s="27" t="s">
         <v>61</v>
@@ -1563,7 +1635,7 @@
       <c r="C81" s="25"/>
       <c r="D81" s="29"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
       <c r="B82" s="27" t="s">
         <v>62</v>
@@ -1571,7 +1643,7 @@
       <c r="C82" s="25"/>
       <c r="D82" s="29"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="27" t="s">
         <v>63</v>
@@ -1579,7 +1651,7 @@
       <c r="C83" s="25"/>
       <c r="D83" s="29"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="27" t="s">
         <v>64</v>
@@ -1587,7 +1659,7 @@
       <c r="C84" s="25"/>
       <c r="D84" s="29"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="27" t="s">
         <v>65</v>
@@ -1595,7 +1667,7 @@
       <c r="C85" s="25"/>
       <c r="D85" s="29"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="27" t="s">
         <v>66</v>
@@ -1603,7 +1675,7 @@
       <c r="C86" s="25"/>
       <c r="D86" s="29"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="27" t="s">
         <v>67</v>
@@ -1611,7 +1683,7 @@
       <c r="C87" s="25"/>
       <c r="D87" s="29"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="33" t="s">
         <v>68</v>
       </c>
@@ -1621,20 +1693,55 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C91" s="32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" s="18"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A88:C88"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A47:C47"/>
@@ -1651,41 +1758,6 @@
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A52:C52"/>
     <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.47244094488188981" bottom="0.43307086614173229" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="63" fitToHeight="10" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
modified:   Projet-Site Web-Grille de planification.xlsx
</commit_message>
<xml_diff>
--- a/Projet-Site Web-Grille de planification.xlsx
+++ b/Projet-Site Web-Grille de planification.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
   <si>
     <t>Grille d'analyse pour le développement d'un site web</t>
   </si>
@@ -94,14 +94,6 @@
     <t>Quels actions, est-ce que le client désire que les internautes fassent au site web?</t>
   </si>
   <si>
-    <t>(  )  Appeler le client
-(  )  Envoyer un courriel
-(  )  Remplir un formulaire de contact
-( )  Faire des recherches dans le site
-(  )  Acheter des produits
-(  )  Joindre une liste de diffusion</t>
-  </si>
-  <si>
     <t>Les produits/services du client</t>
   </si>
   <si>
@@ -123,18 +115,12 @@
     <t>Quelle est la clientèle cible du client?</t>
   </si>
   <si>
-    <t>Gens d’affaires (  )          Consommateurs (  )</t>
-  </si>
-  <si>
     <t>Pour des gens d'affaires, quel genre d’entreprise représentent-ils?</t>
   </si>
   <si>
     <t xml:space="preserve">Pour des gens d'affaires, quelle taille d'entreprise représentent-ils? </t>
   </si>
   <si>
-    <t>Petite (  )          Moyenne (  )          Grande (  )</t>
-  </si>
-  <si>
     <t>Pour des consommateurs, dans quel groupe d’âge se situent-ils?</t>
   </si>
   <si>
@@ -142,9 +128,6 @@
   </si>
   <si>
     <t>Est-ce que le site web est destiné pour un marché local ou international?</t>
-  </si>
-  <si>
-    <t>Local (  )          International (  )</t>
   </si>
   <si>
     <t>Dans quelle langue(s) le site devra-t'il être affiché?</t>
@@ -186,10 +169,6 @@
   </si>
   <si>
     <t>Est-ce que le client a des couleurs/motifs en tête pour le site web?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui (  )           Non (  )
-</t>
   </si>
   <si>
     <t>Est-ce qu'il y a d'autre choses spécifiques que le client veut voir dans son site?</t>
@@ -327,6 +306,33 @@
   </si>
   <si>
     <t>../html/contact.html</t>
+  </si>
+  <si>
+    <t>(  )  Appeler le client
+(  )  Envoyer un courriel
+( X )  Remplir un formulaire de contact
+( )  Faire des recherches dans le site
+( X )  Acheter des produits
+(  )  Joindre une liste de diffusion</t>
+  </si>
+  <si>
+    <t>Gens d’affaires (  )          Consommateurs (X  )</t>
+  </si>
+  <si>
+    <t>Petite (X  )          Moyenne ( X)          Grande (  )</t>
+  </si>
+  <si>
+    <t>Local (  )          International ( X  )</t>
+  </si>
+  <si>
+    <t>Oui ( X )           Non (  )</t>
+  </si>
+  <si>
+    <t>Vanderlay Industries - spécialisée dans la production et la vente de produits en latex de haute qualité,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oui (  )           Non ( X )
+</t>
   </si>
 </sst>
 </file>
@@ -646,41 +652,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -964,8 +970,8 @@
   </sheetPr>
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,20 +984,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -1000,7 +1006,7 @@
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1018,7 +1024,7 @@
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
       <c r="D7" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1036,7 +1042,7 @@
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
       <c r="D9" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,53 +1052,53 @@
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
       <c r="D10" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="41"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="41"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,27 +1110,27 @@
       <c r="D16" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
       <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1134,7 +1140,7 @@
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="6" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,16 +1156,16 @@
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
+      <c r="A25" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
     </row>
     <row r="26" spans="1:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
@@ -1167,7 +1173,7 @@
     </row>
     <row r="27" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
@@ -1175,7 +1181,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
@@ -1183,7 +1189,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
@@ -1204,27 +1210,27 @@
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="36"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
       <c r="D33" s="5" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="7"/>
@@ -1232,17 +1238,17 @@
     <row r="35" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="5" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="7"/>
@@ -1250,24 +1256,24 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
       <c r="B37" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
       <c r="D38" s="5" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
@@ -1280,45 +1286,45 @@
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
+      <c r="A42" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
+        <v>33</v>
+      </c>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
       <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
+      <c r="A44" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
+      <c r="A45" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
@@ -1326,7 +1332,7 @@
     </row>
     <row r="47" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
@@ -1343,31 +1349,31 @@
       <c r="C49" s="19"/>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
+      <c r="A50" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
     </row>
     <row r="51" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B51" s="33"/>
       <c r="C51" s="33"/>
       <c r="D51" s="3" t="s">
-        <v>12</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
       <c r="D52" s="28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1376,10 +1382,10 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,10 +1394,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1400,10 +1406,10 @@
         <v>3</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1412,10 +1418,10 @@
         <v>4</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1424,10 +1430,10 @@
         <v>5</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1436,10 +1442,10 @@
         <v>6</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1448,10 +1454,10 @@
         <v>7</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1494,25 +1500,27 @@
     </row>
     <row r="65" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B65" s="33"/>
       <c r="C65" s="33"/>
-      <c r="D65" s="6"/>
+      <c r="D65" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="66" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="33" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B66" s="33"/>
       <c r="C66" s="33"/>
       <c r="D66" s="30" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="33" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B67" s="33"/>
       <c r="C67" s="33"/>
@@ -1529,46 +1537,46 @@
       <c r="C69" s="19"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
+      <c r="A70" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
     </row>
     <row r="71" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B71" s="40"/>
-      <c r="C71" s="41"/>
+      <c r="A71" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" s="37"/>
+      <c r="C71" s="38"/>
       <c r="D71" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B72" s="40"/>
-      <c r="C72" s="41"/>
+      <c r="A72" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B72" s="37"/>
+      <c r="C72" s="38"/>
       <c r="D72" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="40"/>
-      <c r="C73" s="41"/>
+      <c r="A73" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="37"/>
+      <c r="C73" s="38"/>
       <c r="D73" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="33" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B74" s="33"/>
       <c r="C74" s="33"/>
@@ -1578,7 +1586,7 @@
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="33" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B75" s="33"/>
       <c r="C75" s="33"/>
@@ -1588,7 +1596,7 @@
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="33" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B76" s="33"/>
       <c r="C76" s="33"/>
@@ -1602,16 +1610,16 @@
       <c r="C77" s="19"/>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B78" s="37"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
+      <c r="A78" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="35"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B79" s="33"/>
       <c r="C79" s="33"/>
@@ -1619,18 +1627,18 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="33" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B80" s="33"/>
       <c r="C80" s="33"/>
       <c r="D80" s="29" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="22"/>
       <c r="B81" s="27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C81" s="25"/>
       <c r="D81" s="29"/>
@@ -1638,7 +1646,7 @@
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="22"/>
       <c r="B82" s="27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C82" s="25"/>
       <c r="D82" s="29"/>
@@ -1646,7 +1654,7 @@
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="22"/>
       <c r="B83" s="27" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C83" s="25"/>
       <c r="D83" s="29"/>
@@ -1654,7 +1662,7 @@
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="22"/>
       <c r="B84" s="27" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C84" s="25"/>
       <c r="D84" s="29"/>
@@ -1662,7 +1670,7 @@
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="22"/>
       <c r="B85" s="27" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="29"/>
@@ -1670,7 +1678,7 @@
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="22"/>
       <c r="B86" s="27" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C86" s="25"/>
       <c r="D86" s="29"/>
@@ -1678,24 +1686,24 @@
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
       <c r="B87" s="27" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C87" s="25"/>
       <c r="D87" s="29"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="33" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B88" s="33"/>
       <c r="C88" s="33"/>
       <c r="D88" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C91" s="32" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
@@ -1707,25 +1715,22 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A88:C88"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A71:C71"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A21:C21"/>
@@ -1742,22 +1747,25 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A88:C88"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.47244094488188981" bottom="0.43307086614173229" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="63" fitToHeight="10" orientation="portrait" r:id="rId1"/>

</xml_diff>